<commit_message>
UML Main Charachter Added
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jaar 2\Gamelab2\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jaar 2\Gamelab2\Development\Development Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -469,18 +469,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -488,6 +484,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -770,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +802,7 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -835,34 +840,34 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
@@ -873,34 +878,34 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>72</v>
       </c>
       <c r="K5" t="s">
@@ -911,34 +916,34 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>73</v>
       </c>
       <c r="K6" t="s">
@@ -946,31 +951,31 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="26" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>74</v>
       </c>
       <c r="K7" t="s">
@@ -978,25 +983,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="20" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="8" t="s">
         <v>76</v>
       </c>
       <c r="K8" t="s">
@@ -1004,22 +1009,22 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="16" t="s">
         <v>82</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="8" t="s">
         <v>77</v>
       </c>
       <c r="K9" t="s">
@@ -1027,16 +1032,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="31" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="8" t="s">
         <v>81</v>
       </c>
       <c r="K10" t="s">
@@ -1044,7 +1049,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="29" t="s">
         <v>59</v>
       </c>
       <c r="K11" t="s">
@@ -1052,7 +1057,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="29" t="s">
         <v>50</v>
       </c>
       <c r="K12" t="s">
@@ -1060,7 +1065,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="31" t="s">
         <v>52</v>
       </c>
       <c r="K13" t="s">
@@ -1099,6 +1104,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1212,12 +1223,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1228,6 +1233,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1243,21 +1263,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
UML en Script Overzicht update bij Weapons
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
   <si>
     <t>Main Charachter</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Enemy base class</t>
+  </si>
+  <si>
+    <t>Weapon Manager</t>
   </si>
 </sst>
 </file>
@@ -775,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,6 +1055,9 @@
       <c r="A11" s="29" t="s">
         <v>59</v>
       </c>
+      <c r="G11" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="K11" t="s">
         <v>49</v>
       </c>
@@ -1104,6 +1110,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1217,12 +1229,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1233,6 +1239,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1248,21 +1269,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update UML met Animations en Pickups
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -461,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -470,7 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -778,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +804,7 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -843,34 +842,34 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
@@ -881,34 +880,34 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>72</v>
       </c>
       <c r="K5" t="s">
@@ -919,34 +918,34 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>73</v>
       </c>
       <c r="K6" t="s">
@@ -954,31 +953,31 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>74</v>
       </c>
       <c r="K7" t="s">
@@ -986,25 +985,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>76</v>
       </c>
       <c r="K8" t="s">
@@ -1012,22 +1011,22 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>77</v>
       </c>
       <c r="K9" t="s">
@@ -1035,16 +1034,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>81</v>
       </c>
       <c r="K10" t="s">
@@ -1052,10 +1051,10 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>85</v>
       </c>
       <c r="K11" t="s">
@@ -1063,7 +1062,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>50</v>
       </c>
       <c r="K12" t="s">
@@ -1071,7 +1070,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>52</v>
       </c>
       <c r="K13" t="s">
@@ -1110,6 +1109,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1223,12 +1228,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1239,6 +1238,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1254,21 +1268,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Balancer finished + scripting overzicht
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gamelab2\Development\Development Algemeen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
   </bookViews>
@@ -18,8 +13,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Danial</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Danial:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Enemy ammo drop
+randomrange voor elk type enemy
+list ammo type</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>Main Charachter</t>
   </si>
@@ -280,13 +311,22 @@
   </si>
   <si>
     <t>PowerFistBar</t>
+  </si>
+  <si>
+    <t>Recoil</t>
+  </si>
+  <si>
+    <t>Particles</t>
+  </si>
+  <si>
+    <t>Explosive damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +349,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -477,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -487,7 +540,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -517,7 +569,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -787,43 +839,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="4" width="28.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="29.5546875" customWidth="1"/>
+    <col min="10" max="10" width="34.5546875" customWidth="1"/>
     <col min="11" max="11" width="61" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -861,35 +913,35 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
@@ -899,35 +951,35 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>71</v>
       </c>
       <c r="K5" t="s">
@@ -937,191 +989,199 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>72</v>
       </c>
       <c r="K6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>73</v>
       </c>
       <c r="K7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>84</v>
       </c>
       <c r="K8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="17" t="s">
         <v>75</v>
       </c>
       <c r="K9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="22" t="s">
         <v>79</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>86</v>
       </c>
       <c r="K11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="30" t="s">
+        <v>87</v>
+      </c>
       <c r="K12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>51</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="K13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="30" t="s">
+        <v>89</v>
+      </c>
       <c r="K14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:11" ht="15" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" ht="15" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" ht="15" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
         <v>56</v>
       </c>
@@ -1129,10 +1189,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1246,22 +1322,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1275,27 +1359,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Scripting Overzicht edit + update
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -13,44 +13,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Danial</author>
-  </authors>
-  <commentList>
-    <comment ref="D7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Danial:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Enemy ammo drop
-randomrange voor elk type enemy
-list ammo type</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Main Charachter</t>
   </si>
@@ -314,19 +278,13 @@
   </si>
   <si>
     <t>Recoil</t>
-  </si>
-  <si>
-    <t>Particles</t>
-  </si>
-  <si>
-    <t>Explosive damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,19 +307,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -551,7 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -567,6 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,36 +791,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="4" width="28.5546875" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="29.5546875" customWidth="1"/>
-    <col min="10" max="10" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" customWidth="1"/>
     <col min="11" max="11" width="61" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -913,35 +858,35 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
@@ -951,32 +896,32 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>85</v>
       </c>
       <c r="J5" s="11" t="s">
@@ -989,26 +934,26 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="15" t="s">
@@ -1024,23 +969,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>61</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="28" t="s">
         <v>36</v>
       </c>
       <c r="H7" s="12" t="s">
@@ -1056,17 +1001,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>66</v>
       </c>
       <c r="H8" s="17" t="s">
@@ -1082,20 +1027,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>70</v>
       </c>
       <c r="J9" s="17" t="s">
@@ -1105,83 +1050,77 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>68</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="J10" s="21" t="s">
         <v>79</v>
       </c>
       <c r="K10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>86</v>
       </c>
       <c r="K11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="16" t="s">
         <v>87</v>
       </c>
       <c r="K12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="30" t="s">
-        <v>88</v>
-      </c>
       <c r="K13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G14" s="30" t="s">
-        <v>89</v>
-      </c>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="11:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="11:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="11:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
         <v>56</v>
       </c>
@@ -1189,7 +1128,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Shooting Mummy Sound Done
</commit_message>
<xml_diff>
--- a/Development/Development Algemeen/ScriptingOverzicht.xlsx
+++ b/Development/Development Algemeen/ScriptingOverzicht.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gamelab2\Development\Development Algemeen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
   </bookViews>
@@ -283,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,13 +495,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -509,12 +512,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -784,7 +788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -794,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,31 +866,31 @@
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="31" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
@@ -900,28 +904,28 @@
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="19" t="s">
         <v>85</v>
       </c>
       <c r="J5" s="11" t="s">
@@ -941,25 +945,25 @@
       <c r="B6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>32</v>
       </c>
       <c r="J6" s="11" t="s">
@@ -973,28 +977,28 @@
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="29" t="s">
         <v>59</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>73</v>
       </c>
       <c r="K7" t="s">
@@ -1005,19 +1009,19 @@
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>42</v>
       </c>
       <c r="J8" s="11" t="s">
@@ -1031,19 +1035,19 @@
       <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="19" t="s">
         <v>75</v>
       </c>
       <c r="K9" t="s">
@@ -1054,13 +1058,13 @@
       <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="19" t="s">
         <v>79</v>
       </c>
       <c r="K10" t="s">
@@ -1071,10 +1075,10 @@
       <c r="A11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>86</v>
       </c>
       <c r="K11" t="s">
@@ -1085,7 +1089,7 @@
       <c r="A12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>87</v>
       </c>
       <c r="K12" t="s">
@@ -1138,15 +1142,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1260,6 +1255,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{369E1C53-EC6C-46EA-88F2-558DE2E1BF5D}">
   <ds:schemaRefs>
@@ -1276,14 +1280,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1297,4 +1293,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>